<commit_message>
python reading from uploaded sheets and accepting xls
</commit_message>
<xml_diff>
--- a/public/python/planilhas/Disciplinas.xlsx
+++ b/public/python/planilhas/Disciplinas.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cauel\OneDrive\Desktop\Udesc-Scheduling\storage\app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cauel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42E986C-A06E-42F3-BD54-85012BB6F770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37008782-C874-4B84-B17E-4F12DE8D7D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Template Disciplinas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="134">
   <si>
     <t>Nome-Chave Professor</t>
   </si>
@@ -427,7 +438,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -478,14 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -505,10 +509,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,10 +524,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -621,17 +625,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="3">
-    <tableStyle name="Template Disciplinas-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Template Disciplinas-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
       <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="Template Disciplinas-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Template Disciplinas-style 2" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle name="Template Disciplinas-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="Template Disciplinas-style 3" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -649,55 +653,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:F252" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:F252" headerRowCount="0">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
+    <tableColumn id="6" name="Column6"/>
   </tableColumns>
   <tableStyleInfo name="Template Disciplinas-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="G1:I252" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="G1:I252" headerRowCount="0">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
   </tableColumns>
   <tableStyleInfo name="Template Disciplinas-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="J1:N252" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_3" displayName="Table_3" ref="J1:N252" headerRowCount="0">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column5"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
   </tableColumns>
   <tableStyleInfo name="Template Disciplinas-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
@@ -898,14 +887,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1517,9 +1506,7 @@
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="8"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -2008,9 +1995,7 @@
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="H29" s="6"/>
       <c r="I29" s="8"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -2084,9 +2069,7 @@
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="H31" s="6"/>
       <c r="I31" s="8"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>

</xml_diff>

<commit_message>
Fluxo de Sucesso e Erro
</commit_message>
<xml_diff>
--- a/public/python/planilhas/Disciplinas.xlsx
+++ b/public/python/planilhas/Disciplinas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cauel\OneDrive\Desktop\Udesc-Scheduling\storage\app\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cauel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42E986C-A06E-42F3-BD54-85012BB6F770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5B1E97-C446-450A-B56C-62B7E60693F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Disciplinas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="132">
   <si>
     <t>Nome-Chave Professor</t>
   </si>
@@ -416,12 +416,6 @@
   </si>
   <si>
     <t>Melhoria de Processo de Software</t>
-  </si>
-  <si>
-    <t>QUI;SEX</t>
-  </si>
-  <si>
-    <t>SEG;TER</t>
   </si>
 </sst>
 </file>
@@ -904,29 +898,29 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" customWidth="1"/>
-    <col min="7" max="7" width="90.88671875" customWidth="1"/>
-    <col min="8" max="8" width="53.77734375" customWidth="1"/>
-    <col min="9" max="9" width="2.77734375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="90.85546875" customWidth="1"/>
+    <col min="8" max="8" width="53.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
     <col min="10" max="10" width="87" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
     <col min="12" max="12" width="78" customWidth="1"/>
-    <col min="13" max="13" width="6.88671875" customWidth="1"/>
-    <col min="14" max="14" width="2.77734375" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +969,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1012,7 +1006,7 @@
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1043,7 @@
       <c r="X3" s="10"/>
       <c r="Y3" s="10"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1066,9 +1060,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="8"/>
       <c r="J4" s="6"/>
@@ -1088,7 +1080,7 @@
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1125,7 +1117,7 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>80</v>
       </c>
@@ -1162,7 +1154,7 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
     </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
@@ -1199,7 +1191,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>26</v>
       </c>
@@ -1236,7 +1228,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1273,7 +1265,7 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>26</v>
       </c>
@@ -1310,7 +1302,7 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>36</v>
       </c>
@@ -1347,7 +1339,7 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -1364,9 +1356,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="8"/>
       <c r="J12" s="6"/>
@@ -1386,7 +1376,7 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -1403,9 +1393,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="8"/>
       <c r="J13" s="6"/>
@@ -1425,7 +1413,7 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1450,7 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>47</v>
       </c>
@@ -1499,7 +1487,7 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>26</v>
       </c>
@@ -1538,7 +1526,7 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
     </row>
-    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>52</v>
       </c>
@@ -1575,7 +1563,7 @@
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
     </row>
-    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
@@ -1612,7 +1600,7 @@
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
@@ -1629,9 +1617,7 @@
         <v>13</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="8"/>
       <c r="J19" s="6"/>
@@ -1651,7 +1637,7 @@
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>42</v>
       </c>
@@ -1668,9 +1654,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="8"/>
       <c r="J20" s="6"/>
@@ -1690,7 +1674,7 @@
       <c r="X20" s="10"/>
       <c r="Y20" s="10"/>
     </row>
-    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
@@ -1707,9 +1691,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="8"/>
-      <c r="G21" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="8"/>
       <c r="J21" s="6"/>
@@ -1729,7 +1711,7 @@
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
     </row>
-    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -1766,7 +1748,7 @@
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
     </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>26</v>
       </c>
@@ -1803,7 +1785,7 @@
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>47</v>
       </c>
@@ -1840,7 +1822,7 @@
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
     </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>69</v>
       </c>
@@ -1877,7 +1859,7 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>47</v>
       </c>
@@ -1914,7 +1896,7 @@
       <c r="X26" s="10"/>
       <c r="Y26" s="10"/>
     </row>
-    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>75</v>
       </c>
@@ -1951,7 +1933,7 @@
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
     </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>17</v>
       </c>
@@ -1968,9 +1950,7 @@
         <v>13</v>
       </c>
       <c r="F28" s="8"/>
-      <c r="G28" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="8"/>
       <c r="J28" s="6"/>
@@ -1990,7 +1970,7 @@
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
     </row>
-    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>80</v>
       </c>
@@ -2029,7 +2009,7 @@
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
     </row>
-    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>23</v>
       </c>
@@ -2066,7 +2046,7 @@
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
     </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>69</v>
       </c>
@@ -2105,7 +2085,7 @@
       <c r="X31" s="10"/>
       <c r="Y31" s="10"/>
     </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2122,7 @@
       <c r="X32" s="10"/>
       <c r="Y32" s="10"/>
     </row>
-    <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
@@ -2159,9 +2139,7 @@
         <v>13</v>
       </c>
       <c r="F33" s="8"/>
-      <c r="G33" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="8"/>
       <c r="J33" s="6"/>
@@ -2181,7 +2159,7 @@
       <c r="X33" s="10"/>
       <c r="Y33" s="10"/>
     </row>
-    <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>91</v>
       </c>
@@ -2218,7 +2196,7 @@
       <c r="X34" s="10"/>
       <c r="Y34" s="10"/>
     </row>
-    <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>20</v>
       </c>
@@ -2255,7 +2233,7 @@
       <c r="X35" s="10"/>
       <c r="Y35" s="10"/>
     </row>
-    <row r="36" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>20</v>
       </c>
@@ -2292,7 +2270,7 @@
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
     </row>
-    <row r="37" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>80</v>
       </c>
@@ -2329,7 +2307,7 @@
       <c r="X37" s="10"/>
       <c r="Y37" s="10"/>
     </row>
-    <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>42</v>
       </c>
@@ -2346,9 +2324,7 @@
         <v>13</v>
       </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="8"/>
       <c r="J38" s="6"/>
@@ -2368,7 +2344,7 @@
       <c r="X38" s="10"/>
       <c r="Y38" s="10"/>
     </row>
-    <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>114</v>
       </c>
@@ -2405,7 +2381,7 @@
       <c r="X39" s="10"/>
       <c r="Y39" s="10"/>
     </row>
-    <row r="40" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>69</v>
       </c>
@@ -2442,7 +2418,7 @@
       <c r="X40" s="10"/>
       <c r="Y40" s="10"/>
     </row>
-    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>36</v>
       </c>
@@ -2479,7 +2455,7 @@
       <c r="X41" s="10"/>
       <c r="Y41" s="10"/>
     </row>
-    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>20</v>
       </c>
@@ -2516,7 +2492,7 @@
       <c r="X42" s="10"/>
       <c r="Y42" s="10"/>
     </row>
-    <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>91</v>
       </c>
@@ -2553,7 +2529,7 @@
       <c r="X43" s="10"/>
       <c r="Y43" s="10"/>
     </row>
-    <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>20</v>
       </c>
@@ -2590,7 +2566,7 @@
       <c r="X44" s="10"/>
       <c r="Y44" s="10"/>
     </row>
-    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>114</v>
       </c>
@@ -2627,7 +2603,7 @@
       <c r="X45" s="10"/>
       <c r="Y45" s="10"/>
     </row>
-    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>91</v>
       </c>
@@ -2664,7 +2640,7 @@
       <c r="X46" s="10"/>
       <c r="Y46" s="10"/>
     </row>
-    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
@@ -2701,7 +2677,7 @@
       <c r="X47" s="10"/>
       <c r="Y47" s="10"/>
     </row>
-    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>121</v>
       </c>
@@ -2738,7 +2714,7 @@
       <c r="X48" s="10"/>
       <c r="Y48" s="10"/>
     </row>
-    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>36</v>
       </c>
@@ -2775,7 +2751,7 @@
       <c r="X49" s="10"/>
       <c r="Y49" s="10"/>
     </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>42</v>
       </c>
@@ -2792,9 +2768,7 @@
         <v>13</v>
       </c>
       <c r="F50" s="8"/>
-      <c r="G50" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="8"/>
       <c r="J50" s="6"/>
@@ -2814,7 +2788,7 @@
       <c r="X50" s="10"/>
       <c r="Y50" s="10"/>
     </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>17</v>
       </c>
@@ -2831,9 +2805,7 @@
         <v>13</v>
       </c>
       <c r="F51" s="8"/>
-      <c r="G51" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="8"/>
       <c r="J51" s="6"/>
@@ -2853,7 +2825,7 @@
       <c r="X51" s="10"/>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>36</v>
       </c>
@@ -2890,7 +2862,7 @@
       <c r="X52" s="10"/>
       <c r="Y52" s="10"/>
     </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -2917,7 +2889,7 @@
       <c r="X53" s="10"/>
       <c r="Y53" s="10"/>
     </row>
-    <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -2944,7 +2916,7 @@
       <c r="X54" s="10"/>
       <c r="Y54" s="10"/>
     </row>
-    <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -2971,7 +2943,7 @@
       <c r="X55" s="10"/>
       <c r="Y55" s="10"/>
     </row>
-    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -2998,7 +2970,7 @@
       <c r="X56" s="10"/>
       <c r="Y56" s="10"/>
     </row>
-    <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -3025,7 +2997,7 @@
       <c r="X57" s="10"/>
       <c r="Y57" s="10"/>
     </row>
-    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -3052,7 +3024,7 @@
       <c r="X58" s="10"/>
       <c r="Y58" s="10"/>
     </row>
-    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -3079,7 +3051,7 @@
       <c r="X59" s="10"/>
       <c r="Y59" s="10"/>
     </row>
-    <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -3106,7 +3078,7 @@
       <c r="X60" s="10"/>
       <c r="Y60" s="10"/>
     </row>
-    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -3133,7 +3105,7 @@
       <c r="X61" s="10"/>
       <c r="Y61" s="10"/>
     </row>
-    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -3160,7 +3132,7 @@
       <c r="X62" s="10"/>
       <c r="Y62" s="10"/>
     </row>
-    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -3187,7 +3159,7 @@
       <c r="X63" s="10"/>
       <c r="Y63" s="10"/>
     </row>
-    <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -3214,7 +3186,7 @@
       <c r="X64" s="10"/>
       <c r="Y64" s="10"/>
     </row>
-    <row r="65" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -3241,7 +3213,7 @@
       <c r="X65" s="10"/>
       <c r="Y65" s="10"/>
     </row>
-    <row r="66" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -3268,7 +3240,7 @@
       <c r="X66" s="10"/>
       <c r="Y66" s="10"/>
     </row>
-    <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
@@ -3295,7 +3267,7 @@
       <c r="X67" s="10"/>
       <c r="Y67" s="10"/>
     </row>
-    <row r="68" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="15"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -3322,7 +3294,7 @@
       <c r="X68" s="10"/>
       <c r="Y68" s="10"/>
     </row>
-    <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
@@ -3349,7 +3321,7 @@
       <c r="X69" s="10"/>
       <c r="Y69" s="10"/>
     </row>
-    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="15"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -3376,7 +3348,7 @@
       <c r="X70" s="10"/>
       <c r="Y70" s="10"/>
     </row>
-    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="15"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
@@ -3403,7 +3375,7 @@
       <c r="X71" s="10"/>
       <c r="Y71" s="10"/>
     </row>
-    <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -3430,7 +3402,7 @@
       <c r="X72" s="10"/>
       <c r="Y72" s="10"/>
     </row>
-    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -3457,7 +3429,7 @@
       <c r="X73" s="10"/>
       <c r="Y73" s="10"/>
     </row>
-    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -3484,7 +3456,7 @@
       <c r="X74" s="10"/>
       <c r="Y74" s="10"/>
     </row>
-    <row r="75" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="15"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -3511,7 +3483,7 @@
       <c r="X75" s="10"/>
       <c r="Y75" s="10"/>
     </row>
-    <row r="76" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -3538,7 +3510,7 @@
       <c r="X76" s="10"/>
       <c r="Y76" s="10"/>
     </row>
-    <row r="77" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="15"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -3565,7 +3537,7 @@
       <c r="X77" s="10"/>
       <c r="Y77" s="10"/>
     </row>
-    <row r="78" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -3592,7 +3564,7 @@
       <c r="X78" s="10"/>
       <c r="Y78" s="10"/>
     </row>
-    <row r="79" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -3619,7 +3591,7 @@
       <c r="X79" s="10"/>
       <c r="Y79" s="10"/>
     </row>
-    <row r="80" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -3646,7 +3618,7 @@
       <c r="X80" s="10"/>
       <c r="Y80" s="10"/>
     </row>
-    <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="15"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
@@ -3673,7 +3645,7 @@
       <c r="X81" s="10"/>
       <c r="Y81" s="10"/>
     </row>
-    <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -3700,7 +3672,7 @@
       <c r="X82" s="10"/>
       <c r="Y82" s="10"/>
     </row>
-    <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="15"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -3727,7 +3699,7 @@
       <c r="X83" s="10"/>
       <c r="Y83" s="10"/>
     </row>
-    <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -3754,7 +3726,7 @@
       <c r="X84" s="10"/>
       <c r="Y84" s="10"/>
     </row>
-    <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="15"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -3781,7 +3753,7 @@
       <c r="X85" s="10"/>
       <c r="Y85" s="10"/>
     </row>
-    <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -3808,7 +3780,7 @@
       <c r="X86" s="10"/>
       <c r="Y86" s="10"/>
     </row>
-    <row r="87" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="15"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
@@ -3835,7 +3807,7 @@
       <c r="X87" s="10"/>
       <c r="Y87" s="10"/>
     </row>
-    <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -3862,7 +3834,7 @@
       <c r="X88" s="10"/>
       <c r="Y88" s="10"/>
     </row>
-    <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -3889,7 +3861,7 @@
       <c r="X89" s="10"/>
       <c r="Y89" s="10"/>
     </row>
-    <row r="90" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -3916,7 +3888,7 @@
       <c r="X90" s="10"/>
       <c r="Y90" s="10"/>
     </row>
-    <row r="91" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="15"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -3943,7 +3915,7 @@
       <c r="X91" s="10"/>
       <c r="Y91" s="10"/>
     </row>
-    <row r="92" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -3970,7 +3942,7 @@
       <c r="X92" s="10"/>
       <c r="Y92" s="10"/>
     </row>
-    <row r="93" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
@@ -3997,7 +3969,7 @@
       <c r="X93" s="10"/>
       <c r="Y93" s="10"/>
     </row>
-    <row r="94" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="15"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -4024,7 +3996,7 @@
       <c r="X94" s="10"/>
       <c r="Y94" s="10"/>
     </row>
-    <row r="95" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="15"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
@@ -4051,7 +4023,7 @@
       <c r="X95" s="10"/>
       <c r="Y95" s="10"/>
     </row>
-    <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -4078,7 +4050,7 @@
       <c r="X96" s="10"/>
       <c r="Y96" s="10"/>
     </row>
-    <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -4105,7 +4077,7 @@
       <c r="X97" s="10"/>
       <c r="Y97" s="10"/>
     </row>
-    <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="15"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -4132,7 +4104,7 @@
       <c r="X98" s="10"/>
       <c r="Y98" s="10"/>
     </row>
-    <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -4159,7 +4131,7 @@
       <c r="X99" s="10"/>
       <c r="Y99" s="10"/>
     </row>
-    <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
@@ -4186,7 +4158,7 @@
       <c r="X100" s="10"/>
       <c r="Y100" s="10"/>
     </row>
-    <row r="101" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -4213,7 +4185,7 @@
       <c r="X101" s="10"/>
       <c r="Y101" s="10"/>
     </row>
-    <row r="102" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
@@ -4240,7 +4212,7 @@
       <c r="X102" s="10"/>
       <c r="Y102" s="10"/>
     </row>
-    <row r="103" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
@@ -4267,7 +4239,7 @@
       <c r="X103" s="10"/>
       <c r="Y103" s="10"/>
     </row>
-    <row r="104" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
@@ -4294,7 +4266,7 @@
       <c r="X104" s="10"/>
       <c r="Y104" s="10"/>
     </row>
-    <row r="105" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="15"/>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
@@ -4321,7 +4293,7 @@
       <c r="X105" s="10"/>
       <c r="Y105" s="10"/>
     </row>
-    <row r="106" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="15"/>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
@@ -4348,7 +4320,7 @@
       <c r="X106" s="10"/>
       <c r="Y106" s="10"/>
     </row>
-    <row r="107" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="15"/>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
@@ -4375,7 +4347,7 @@
       <c r="X107" s="10"/>
       <c r="Y107" s="10"/>
     </row>
-    <row r="108" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
@@ -4402,7 +4374,7 @@
       <c r="X108" s="10"/>
       <c r="Y108" s="10"/>
     </row>
-    <row r="109" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
@@ -4429,7 +4401,7 @@
       <c r="X109" s="10"/>
       <c r="Y109" s="10"/>
     </row>
-    <row r="110" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="15"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
@@ -4456,7 +4428,7 @@
       <c r="X110" s="10"/>
       <c r="Y110" s="10"/>
     </row>
-    <row r="111" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="15"/>
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
@@ -4483,7 +4455,7 @@
       <c r="X111" s="10"/>
       <c r="Y111" s="10"/>
     </row>
-    <row r="112" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="15"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
@@ -4510,7 +4482,7 @@
       <c r="X112" s="10"/>
       <c r="Y112" s="10"/>
     </row>
-    <row r="113" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="15"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
@@ -4537,7 +4509,7 @@
       <c r="X113" s="10"/>
       <c r="Y113" s="10"/>
     </row>
-    <row r="114" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="15"/>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
@@ -4564,7 +4536,7 @@
       <c r="X114" s="10"/>
       <c r="Y114" s="10"/>
     </row>
-    <row r="115" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="15"/>
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>
@@ -4591,7 +4563,7 @@
       <c r="X115" s="10"/>
       <c r="Y115" s="10"/>
     </row>
-    <row r="116" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="15"/>
       <c r="B116" s="10"/>
       <c r="C116" s="10"/>
@@ -4618,7 +4590,7 @@
       <c r="X116" s="10"/>
       <c r="Y116" s="10"/>
     </row>
-    <row r="117" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="15"/>
       <c r="B117" s="10"/>
       <c r="C117" s="10"/>
@@ -4645,7 +4617,7 @@
       <c r="X117" s="10"/>
       <c r="Y117" s="10"/>
     </row>
-    <row r="118" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="15"/>
       <c r="B118" s="10"/>
       <c r="C118" s="10"/>
@@ -4672,7 +4644,7 @@
       <c r="X118" s="10"/>
       <c r="Y118" s="10"/>
     </row>
-    <row r="119" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="15"/>
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
@@ -4699,7 +4671,7 @@
       <c r="X119" s="10"/>
       <c r="Y119" s="10"/>
     </row>
-    <row r="120" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="15"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -4726,7 +4698,7 @@
       <c r="X120" s="10"/>
       <c r="Y120" s="10"/>
     </row>
-    <row r="121" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="15"/>
       <c r="B121" s="10"/>
       <c r="C121" s="10"/>
@@ -4753,7 +4725,7 @@
       <c r="X121" s="10"/>
       <c r="Y121" s="10"/>
     </row>
-    <row r="122" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="15"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
@@ -4780,7 +4752,7 @@
       <c r="X122" s="10"/>
       <c r="Y122" s="10"/>
     </row>
-    <row r="123" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="15"/>
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
@@ -4807,7 +4779,7 @@
       <c r="X123" s="10"/>
       <c r="Y123" s="10"/>
     </row>
-    <row r="124" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="15"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -4834,7 +4806,7 @@
       <c r="X124" s="10"/>
       <c r="Y124" s="10"/>
     </row>
-    <row r="125" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="15"/>
       <c r="B125" s="10"/>
       <c r="C125" s="10"/>
@@ -4861,7 +4833,7 @@
       <c r="X125" s="10"/>
       <c r="Y125" s="10"/>
     </row>
-    <row r="126" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="15"/>
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
@@ -4888,7 +4860,7 @@
       <c r="X126" s="10"/>
       <c r="Y126" s="10"/>
     </row>
-    <row r="127" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="15"/>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
@@ -4915,7 +4887,7 @@
       <c r="X127" s="10"/>
       <c r="Y127" s="10"/>
     </row>
-    <row r="128" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="15"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -4942,7 +4914,7 @@
       <c r="X128" s="10"/>
       <c r="Y128" s="10"/>
     </row>
-    <row r="129" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="15"/>
       <c r="B129" s="10"/>
       <c r="C129" s="10"/>
@@ -4969,7 +4941,7 @@
       <c r="X129" s="10"/>
       <c r="Y129" s="10"/>
     </row>
-    <row r="130" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="15"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -4996,7 +4968,7 @@
       <c r="X130" s="10"/>
       <c r="Y130" s="10"/>
     </row>
-    <row r="131" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="15"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
@@ -5023,7 +4995,7 @@
       <c r="X131" s="10"/>
       <c r="Y131" s="10"/>
     </row>
-    <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="15"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -5050,7 +5022,7 @@
       <c r="X132" s="10"/>
       <c r="Y132" s="10"/>
     </row>
-    <row r="133" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="15"/>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
@@ -5077,7 +5049,7 @@
       <c r="X133" s="10"/>
       <c r="Y133" s="10"/>
     </row>
-    <row r="134" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="15"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -5104,7 +5076,7 @@
       <c r="X134" s="10"/>
       <c r="Y134" s="10"/>
     </row>
-    <row r="135" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="15"/>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
@@ -5131,7 +5103,7 @@
       <c r="X135" s="10"/>
       <c r="Y135" s="10"/>
     </row>
-    <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="15"/>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -5158,7 +5130,7 @@
       <c r="X136" s="10"/>
       <c r="Y136" s="10"/>
     </row>
-    <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="15"/>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -5185,7 +5157,7 @@
       <c r="X137" s="10"/>
       <c r="Y137" s="10"/>
     </row>
-    <row r="138" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="15"/>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -5212,7 +5184,7 @@
       <c r="X138" s="10"/>
       <c r="Y138" s="10"/>
     </row>
-    <row r="139" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="15"/>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -5239,7 +5211,7 @@
       <c r="X139" s="10"/>
       <c r="Y139" s="10"/>
     </row>
-    <row r="140" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="15"/>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -5266,7 +5238,7 @@
       <c r="X140" s="10"/>
       <c r="Y140" s="10"/>
     </row>
-    <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="15"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -5293,7 +5265,7 @@
       <c r="X141" s="10"/>
       <c r="Y141" s="10"/>
     </row>
-    <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="15"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -5320,7 +5292,7 @@
       <c r="X142" s="10"/>
       <c r="Y142" s="10"/>
     </row>
-    <row r="143" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="15"/>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -5347,7 +5319,7 @@
       <c r="X143" s="10"/>
       <c r="Y143" s="10"/>
     </row>
-    <row r="144" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="15"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -5374,7 +5346,7 @@
       <c r="X144" s="10"/>
       <c r="Y144" s="10"/>
     </row>
-    <row r="145" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="15"/>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
@@ -5401,7 +5373,7 @@
       <c r="X145" s="10"/>
       <c r="Y145" s="10"/>
     </row>
-    <row r="146" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="15"/>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -5428,7 +5400,7 @@
       <c r="X146" s="10"/>
       <c r="Y146" s="10"/>
     </row>
-    <row r="147" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="15"/>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
@@ -5455,7 +5427,7 @@
       <c r="X147" s="10"/>
       <c r="Y147" s="10"/>
     </row>
-    <row r="148" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="15"/>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
@@ -5482,7 +5454,7 @@
       <c r="X148" s="10"/>
       <c r="Y148" s="10"/>
     </row>
-    <row r="149" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="15"/>
       <c r="B149" s="10"/>
       <c r="C149" s="10"/>
@@ -5509,7 +5481,7 @@
       <c r="X149" s="10"/>
       <c r="Y149" s="10"/>
     </row>
-    <row r="150" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="15"/>
       <c r="B150" s="10"/>
       <c r="C150" s="10"/>
@@ -5536,7 +5508,7 @@
       <c r="X150" s="10"/>
       <c r="Y150" s="10"/>
     </row>
-    <row r="151" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="15"/>
       <c r="B151" s="10"/>
       <c r="C151" s="10"/>
@@ -5563,7 +5535,7 @@
       <c r="X151" s="10"/>
       <c r="Y151" s="10"/>
     </row>
-    <row r="152" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="15"/>
       <c r="B152" s="10"/>
       <c r="C152" s="10"/>
@@ -5590,7 +5562,7 @@
       <c r="X152" s="10"/>
       <c r="Y152" s="10"/>
     </row>
-    <row r="153" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="15"/>
       <c r="B153" s="10"/>
       <c r="C153" s="10"/>
@@ -5617,7 +5589,7 @@
       <c r="X153" s="10"/>
       <c r="Y153" s="10"/>
     </row>
-    <row r="154" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="15"/>
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
@@ -5644,7 +5616,7 @@
       <c r="X154" s="10"/>
       <c r="Y154" s="10"/>
     </row>
-    <row r="155" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="15"/>
       <c r="B155" s="10"/>
       <c r="C155" s="10"/>
@@ -5671,7 +5643,7 @@
       <c r="X155" s="10"/>
       <c r="Y155" s="10"/>
     </row>
-    <row r="156" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="15"/>
       <c r="B156" s="10"/>
       <c r="C156" s="10"/>
@@ -5698,7 +5670,7 @@
       <c r="X156" s="10"/>
       <c r="Y156" s="10"/>
     </row>
-    <row r="157" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="15"/>
       <c r="B157" s="10"/>
       <c r="C157" s="10"/>
@@ -5725,7 +5697,7 @@
       <c r="X157" s="10"/>
       <c r="Y157" s="10"/>
     </row>
-    <row r="158" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="15"/>
       <c r="B158" s="10"/>
       <c r="C158" s="10"/>
@@ -5752,7 +5724,7 @@
       <c r="X158" s="10"/>
       <c r="Y158" s="10"/>
     </row>
-    <row r="159" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="15"/>
       <c r="B159" s="10"/>
       <c r="C159" s="10"/>
@@ -5779,7 +5751,7 @@
       <c r="X159" s="10"/>
       <c r="Y159" s="10"/>
     </row>
-    <row r="160" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="15"/>
       <c r="B160" s="10"/>
       <c r="C160" s="10"/>
@@ -5806,7 +5778,7 @@
       <c r="X160" s="10"/>
       <c r="Y160" s="10"/>
     </row>
-    <row r="161" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="15"/>
       <c r="B161" s="10"/>
       <c r="C161" s="10"/>
@@ -5833,7 +5805,7 @@
       <c r="X161" s="10"/>
       <c r="Y161" s="10"/>
     </row>
-    <row r="162" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="15"/>
       <c r="B162" s="10"/>
       <c r="C162" s="10"/>
@@ -5860,7 +5832,7 @@
       <c r="X162" s="10"/>
       <c r="Y162" s="10"/>
     </row>
-    <row r="163" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="15"/>
       <c r="B163" s="10"/>
       <c r="C163" s="10"/>
@@ -5887,7 +5859,7 @@
       <c r="X163" s="10"/>
       <c r="Y163" s="10"/>
     </row>
-    <row r="164" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="15"/>
       <c r="B164" s="10"/>
       <c r="C164" s="10"/>
@@ -5914,7 +5886,7 @@
       <c r="X164" s="10"/>
       <c r="Y164" s="10"/>
     </row>
-    <row r="165" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="15"/>
       <c r="B165" s="10"/>
       <c r="C165" s="10"/>
@@ -5941,7 +5913,7 @@
       <c r="X165" s="10"/>
       <c r="Y165" s="10"/>
     </row>
-    <row r="166" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" s="10"/>
       <c r="C166" s="10"/>
@@ -5968,7 +5940,7 @@
       <c r="X166" s="10"/>
       <c r="Y166" s="10"/>
     </row>
-    <row r="167" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="10"/>
       <c r="C167" s="10"/>
@@ -5995,7 +5967,7 @@
       <c r="X167" s="10"/>
       <c r="Y167" s="10"/>
     </row>
-    <row r="168" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="15"/>
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
@@ -6022,7 +5994,7 @@
       <c r="X168" s="10"/>
       <c r="Y168" s="10"/>
     </row>
-    <row r="169" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="15"/>
       <c r="B169" s="10"/>
       <c r="C169" s="10"/>
@@ -6049,7 +6021,7 @@
       <c r="X169" s="10"/>
       <c r="Y169" s="10"/>
     </row>
-    <row r="170" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="15"/>
       <c r="B170" s="10"/>
       <c r="C170" s="10"/>
@@ -6076,7 +6048,7 @@
       <c r="X170" s="10"/>
       <c r="Y170" s="10"/>
     </row>
-    <row r="171" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="15"/>
       <c r="B171" s="10"/>
       <c r="C171" s="10"/>
@@ -6103,7 +6075,7 @@
       <c r="X171" s="10"/>
       <c r="Y171" s="10"/>
     </row>
-    <row r="172" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="15"/>
       <c r="B172" s="10"/>
       <c r="C172" s="10"/>
@@ -6130,7 +6102,7 @@
       <c r="X172" s="10"/>
       <c r="Y172" s="10"/>
     </row>
-    <row r="173" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="15"/>
       <c r="B173" s="10"/>
       <c r="C173" s="10"/>
@@ -6157,7 +6129,7 @@
       <c r="X173" s="10"/>
       <c r="Y173" s="10"/>
     </row>
-    <row r="174" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="15"/>
       <c r="B174" s="10"/>
       <c r="C174" s="10"/>
@@ -6184,7 +6156,7 @@
       <c r="X174" s="10"/>
       <c r="Y174" s="10"/>
     </row>
-    <row r="175" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="15"/>
       <c r="B175" s="10"/>
       <c r="C175" s="10"/>
@@ -6211,7 +6183,7 @@
       <c r="X175" s="10"/>
       <c r="Y175" s="10"/>
     </row>
-    <row r="176" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="15"/>
       <c r="B176" s="10"/>
       <c r="C176" s="10"/>
@@ -6238,7 +6210,7 @@
       <c r="X176" s="10"/>
       <c r="Y176" s="10"/>
     </row>
-    <row r="177" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="15"/>
       <c r="B177" s="10"/>
       <c r="C177" s="10"/>
@@ -6265,7 +6237,7 @@
       <c r="X177" s="10"/>
       <c r="Y177" s="10"/>
     </row>
-    <row r="178" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="15"/>
       <c r="B178" s="10"/>
       <c r="C178" s="10"/>
@@ -6292,7 +6264,7 @@
       <c r="X178" s="10"/>
       <c r="Y178" s="10"/>
     </row>
-    <row r="179" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="15"/>
       <c r="B179" s="10"/>
       <c r="C179" s="10"/>
@@ -6319,7 +6291,7 @@
       <c r="X179" s="10"/>
       <c r="Y179" s="10"/>
     </row>
-    <row r="180" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="15"/>
       <c r="B180" s="10"/>
       <c r="C180" s="10"/>
@@ -6346,7 +6318,7 @@
       <c r="X180" s="10"/>
       <c r="Y180" s="10"/>
     </row>
-    <row r="181" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="15"/>
       <c r="B181" s="10"/>
       <c r="C181" s="10"/>
@@ -6373,7 +6345,7 @@
       <c r="X181" s="10"/>
       <c r="Y181" s="10"/>
     </row>
-    <row r="182" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="15"/>
       <c r="B182" s="10"/>
       <c r="C182" s="10"/>
@@ -6400,7 +6372,7 @@
       <c r="X182" s="10"/>
       <c r="Y182" s="10"/>
     </row>
-    <row r="183" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="15"/>
       <c r="B183" s="10"/>
       <c r="C183" s="10"/>
@@ -6427,7 +6399,7 @@
       <c r="X183" s="10"/>
       <c r="Y183" s="10"/>
     </row>
-    <row r="184" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="15"/>
       <c r="B184" s="10"/>
       <c r="C184" s="10"/>
@@ -6454,7 +6426,7 @@
       <c r="X184" s="10"/>
       <c r="Y184" s="10"/>
     </row>
-    <row r="185" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="15"/>
       <c r="B185" s="10"/>
       <c r="C185" s="10"/>
@@ -6481,7 +6453,7 @@
       <c r="X185" s="10"/>
       <c r="Y185" s="10"/>
     </row>
-    <row r="186" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="15"/>
       <c r="B186" s="10"/>
       <c r="C186" s="10"/>
@@ -6508,7 +6480,7 @@
       <c r="X186" s="10"/>
       <c r="Y186" s="10"/>
     </row>
-    <row r="187" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="15"/>
       <c r="B187" s="10"/>
       <c r="C187" s="10"/>
@@ -6535,7 +6507,7 @@
       <c r="X187" s="10"/>
       <c r="Y187" s="10"/>
     </row>
-    <row r="188" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="15"/>
       <c r="B188" s="10"/>
       <c r="C188" s="10"/>
@@ -6562,7 +6534,7 @@
       <c r="X188" s="10"/>
       <c r="Y188" s="10"/>
     </row>
-    <row r="189" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="15"/>
       <c r="B189" s="10"/>
       <c r="C189" s="10"/>
@@ -6589,7 +6561,7 @@
       <c r="X189" s="10"/>
       <c r="Y189" s="10"/>
     </row>
-    <row r="190" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="15"/>
       <c r="B190" s="10"/>
       <c r="C190" s="10"/>
@@ -6616,7 +6588,7 @@
       <c r="X190" s="10"/>
       <c r="Y190" s="10"/>
     </row>
-    <row r="191" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="15"/>
       <c r="B191" s="10"/>
       <c r="C191" s="10"/>
@@ -6643,7 +6615,7 @@
       <c r="X191" s="10"/>
       <c r="Y191" s="10"/>
     </row>
-    <row r="192" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="15"/>
       <c r="B192" s="10"/>
       <c r="C192" s="10"/>
@@ -6670,7 +6642,7 @@
       <c r="X192" s="10"/>
       <c r="Y192" s="10"/>
     </row>
-    <row r="193" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="15"/>
       <c r="B193" s="10"/>
       <c r="C193" s="10"/>
@@ -6697,7 +6669,7 @@
       <c r="X193" s="10"/>
       <c r="Y193" s="10"/>
     </row>
-    <row r="194" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="15"/>
       <c r="B194" s="10"/>
       <c r="C194" s="10"/>
@@ -6724,7 +6696,7 @@
       <c r="X194" s="10"/>
       <c r="Y194" s="10"/>
     </row>
-    <row r="195" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="15"/>
       <c r="B195" s="10"/>
       <c r="C195" s="10"/>
@@ -6751,7 +6723,7 @@
       <c r="X195" s="10"/>
       <c r="Y195" s="10"/>
     </row>
-    <row r="196" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="15"/>
       <c r="B196" s="10"/>
       <c r="C196" s="10"/>
@@ -6778,7 +6750,7 @@
       <c r="X196" s="10"/>
       <c r="Y196" s="10"/>
     </row>
-    <row r="197" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="15"/>
       <c r="B197" s="10"/>
       <c r="C197" s="10"/>
@@ -6805,7 +6777,7 @@
       <c r="X197" s="10"/>
       <c r="Y197" s="10"/>
     </row>
-    <row r="198" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="15"/>
       <c r="B198" s="10"/>
       <c r="C198" s="10"/>
@@ -6832,7 +6804,7 @@
       <c r="X198" s="10"/>
       <c r="Y198" s="10"/>
     </row>
-    <row r="199" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="15"/>
       <c r="B199" s="10"/>
       <c r="C199" s="10"/>
@@ -6859,7 +6831,7 @@
       <c r="X199" s="10"/>
       <c r="Y199" s="10"/>
     </row>
-    <row r="200" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="15"/>
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
@@ -6886,7 +6858,7 @@
       <c r="X200" s="10"/>
       <c r="Y200" s="10"/>
     </row>
-    <row r="201" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="15"/>
       <c r="B201" s="10"/>
       <c r="C201" s="10"/>
@@ -6913,7 +6885,7 @@
       <c r="X201" s="10"/>
       <c r="Y201" s="10"/>
     </row>
-    <row r="202" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="15"/>
       <c r="B202" s="10"/>
       <c r="C202" s="10"/>
@@ -6940,7 +6912,7 @@
       <c r="X202" s="10"/>
       <c r="Y202" s="10"/>
     </row>
-    <row r="203" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="15"/>
       <c r="B203" s="10"/>
       <c r="C203" s="10"/>
@@ -6967,7 +6939,7 @@
       <c r="X203" s="10"/>
       <c r="Y203" s="10"/>
     </row>
-    <row r="204" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="15"/>
       <c r="B204" s="10"/>
       <c r="C204" s="10"/>
@@ -6994,7 +6966,7 @@
       <c r="X204" s="10"/>
       <c r="Y204" s="10"/>
     </row>
-    <row r="205" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="15"/>
       <c r="B205" s="10"/>
       <c r="C205" s="10"/>
@@ -7021,7 +6993,7 @@
       <c r="X205" s="10"/>
       <c r="Y205" s="10"/>
     </row>
-    <row r="206" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="15"/>
       <c r="B206" s="10"/>
       <c r="C206" s="10"/>
@@ -7048,7 +7020,7 @@
       <c r="X206" s="10"/>
       <c r="Y206" s="10"/>
     </row>
-    <row r="207" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="15"/>
       <c r="B207" s="10"/>
       <c r="C207" s="10"/>
@@ -7075,7 +7047,7 @@
       <c r="X207" s="10"/>
       <c r="Y207" s="10"/>
     </row>
-    <row r="208" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="15"/>
       <c r="B208" s="10"/>
       <c r="C208" s="10"/>
@@ -7102,7 +7074,7 @@
       <c r="X208" s="10"/>
       <c r="Y208" s="10"/>
     </row>
-    <row r="209" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="15"/>
       <c r="B209" s="10"/>
       <c r="C209" s="10"/>
@@ -7129,7 +7101,7 @@
       <c r="X209" s="10"/>
       <c r="Y209" s="10"/>
     </row>
-    <row r="210" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="15"/>
       <c r="B210" s="10"/>
       <c r="C210" s="10"/>
@@ -7156,7 +7128,7 @@
       <c r="X210" s="10"/>
       <c r="Y210" s="10"/>
     </row>
-    <row r="211" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="15"/>
       <c r="B211" s="10"/>
       <c r="C211" s="10"/>
@@ -7183,7 +7155,7 @@
       <c r="X211" s="10"/>
       <c r="Y211" s="10"/>
     </row>
-    <row r="212" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="15"/>
       <c r="B212" s="10"/>
       <c r="C212" s="10"/>
@@ -7210,7 +7182,7 @@
       <c r="X212" s="10"/>
       <c r="Y212" s="10"/>
     </row>
-    <row r="213" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="15"/>
       <c r="B213" s="10"/>
       <c r="C213" s="10"/>
@@ -7237,7 +7209,7 @@
       <c r="X213" s="10"/>
       <c r="Y213" s="10"/>
     </row>
-    <row r="214" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="15"/>
       <c r="B214" s="10"/>
       <c r="C214" s="10"/>
@@ -7264,7 +7236,7 @@
       <c r="X214" s="10"/>
       <c r="Y214" s="10"/>
     </row>
-    <row r="215" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="15"/>
       <c r="B215" s="10"/>
       <c r="C215" s="10"/>
@@ -7291,7 +7263,7 @@
       <c r="X215" s="10"/>
       <c r="Y215" s="10"/>
     </row>
-    <row r="216" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="15"/>
       <c r="B216" s="10"/>
       <c r="C216" s="10"/>
@@ -7318,7 +7290,7 @@
       <c r="X216" s="10"/>
       <c r="Y216" s="10"/>
     </row>
-    <row r="217" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="15"/>
       <c r="B217" s="10"/>
       <c r="C217" s="10"/>
@@ -7345,7 +7317,7 @@
       <c r="X217" s="10"/>
       <c r="Y217" s="10"/>
     </row>
-    <row r="218" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="15"/>
       <c r="B218" s="10"/>
       <c r="C218" s="10"/>
@@ -7372,7 +7344,7 @@
       <c r="X218" s="10"/>
       <c r="Y218" s="10"/>
     </row>
-    <row r="219" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="15"/>
       <c r="B219" s="10"/>
       <c r="C219" s="10"/>
@@ -7399,7 +7371,7 @@
       <c r="X219" s="10"/>
       <c r="Y219" s="10"/>
     </row>
-    <row r="220" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="15"/>
       <c r="B220" s="10"/>
       <c r="C220" s="10"/>
@@ -7426,7 +7398,7 @@
       <c r="X220" s="10"/>
       <c r="Y220" s="10"/>
     </row>
-    <row r="221" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="15"/>
       <c r="B221" s="10"/>
       <c r="C221" s="10"/>
@@ -7453,7 +7425,7 @@
       <c r="X221" s="10"/>
       <c r="Y221" s="10"/>
     </row>
-    <row r="222" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="15"/>
       <c r="B222" s="10"/>
       <c r="C222" s="10"/>
@@ -7480,7 +7452,7 @@
       <c r="X222" s="10"/>
       <c r="Y222" s="10"/>
     </row>
-    <row r="223" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="15"/>
       <c r="B223" s="10"/>
       <c r="C223" s="10"/>
@@ -7507,7 +7479,7 @@
       <c r="X223" s="10"/>
       <c r="Y223" s="10"/>
     </row>
-    <row r="224" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="15"/>
       <c r="B224" s="10"/>
       <c r="C224" s="10"/>
@@ -7534,7 +7506,7 @@
       <c r="X224" s="10"/>
       <c r="Y224" s="10"/>
     </row>
-    <row r="225" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="15"/>
       <c r="B225" s="10"/>
       <c r="C225" s="10"/>
@@ -7561,7 +7533,7 @@
       <c r="X225" s="10"/>
       <c r="Y225" s="10"/>
     </row>
-    <row r="226" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="15"/>
       <c r="B226" s="10"/>
       <c r="C226" s="10"/>
@@ -7588,7 +7560,7 @@
       <c r="X226" s="10"/>
       <c r="Y226" s="10"/>
     </row>
-    <row r="227" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="15"/>
       <c r="B227" s="10"/>
       <c r="C227" s="10"/>
@@ -7615,7 +7587,7 @@
       <c r="X227" s="10"/>
       <c r="Y227" s="10"/>
     </row>
-    <row r="228" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="15"/>
       <c r="B228" s="10"/>
       <c r="C228" s="10"/>
@@ -7642,7 +7614,7 @@
       <c r="X228" s="10"/>
       <c r="Y228" s="10"/>
     </row>
-    <row r="229" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="15"/>
       <c r="B229" s="10"/>
       <c r="C229" s="10"/>
@@ -7669,7 +7641,7 @@
       <c r="X229" s="10"/>
       <c r="Y229" s="10"/>
     </row>
-    <row r="230" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="15"/>
       <c r="B230" s="10"/>
       <c r="C230" s="10"/>
@@ -7696,7 +7668,7 @@
       <c r="X230" s="10"/>
       <c r="Y230" s="10"/>
     </row>
-    <row r="231" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="15"/>
       <c r="B231" s="10"/>
       <c r="C231" s="10"/>
@@ -7723,7 +7695,7 @@
       <c r="X231" s="10"/>
       <c r="Y231" s="10"/>
     </row>
-    <row r="232" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="15"/>
       <c r="B232" s="10"/>
       <c r="C232" s="10"/>
@@ -7750,7 +7722,7 @@
       <c r="X232" s="10"/>
       <c r="Y232" s="10"/>
     </row>
-    <row r="233" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="15"/>
       <c r="B233" s="10"/>
       <c r="C233" s="10"/>
@@ -7777,7 +7749,7 @@
       <c r="X233" s="10"/>
       <c r="Y233" s="10"/>
     </row>
-    <row r="234" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="15"/>
       <c r="B234" s="10"/>
       <c r="C234" s="10"/>
@@ -7804,7 +7776,7 @@
       <c r="X234" s="10"/>
       <c r="Y234" s="10"/>
     </row>
-    <row r="235" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="15"/>
       <c r="B235" s="10"/>
       <c r="C235" s="10"/>
@@ -7831,7 +7803,7 @@
       <c r="X235" s="10"/>
       <c r="Y235" s="10"/>
     </row>
-    <row r="236" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="15"/>
       <c r="B236" s="10"/>
       <c r="C236" s="10"/>
@@ -7858,7 +7830,7 @@
       <c r="X236" s="10"/>
       <c r="Y236" s="10"/>
     </row>
-    <row r="237" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="15"/>
       <c r="B237" s="10"/>
       <c r="C237" s="10"/>
@@ -7885,7 +7857,7 @@
       <c r="X237" s="10"/>
       <c r="Y237" s="10"/>
     </row>
-    <row r="238" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="15"/>
       <c r="B238" s="10"/>
       <c r="C238" s="10"/>
@@ -7912,7 +7884,7 @@
       <c r="X238" s="10"/>
       <c r="Y238" s="10"/>
     </row>
-    <row r="239" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="15"/>
       <c r="B239" s="10"/>
       <c r="C239" s="10"/>
@@ -7939,7 +7911,7 @@
       <c r="X239" s="10"/>
       <c r="Y239" s="10"/>
     </row>
-    <row r="240" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="15"/>
       <c r="B240" s="10"/>
       <c r="C240" s="10"/>
@@ -7966,7 +7938,7 @@
       <c r="X240" s="10"/>
       <c r="Y240" s="10"/>
     </row>
-    <row r="241" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="15"/>
       <c r="B241" s="10"/>
       <c r="C241" s="10"/>
@@ -7993,7 +7965,7 @@
       <c r="X241" s="10"/>
       <c r="Y241" s="10"/>
     </row>
-    <row r="242" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="15"/>
       <c r="B242" s="10"/>
       <c r="C242" s="10"/>
@@ -8020,7 +7992,7 @@
       <c r="X242" s="10"/>
       <c r="Y242" s="10"/>
     </row>
-    <row r="243" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="15"/>
       <c r="B243" s="10"/>
       <c r="C243" s="10"/>
@@ -8047,7 +8019,7 @@
       <c r="X243" s="10"/>
       <c r="Y243" s="10"/>
     </row>
-    <row r="244" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="15"/>
       <c r="B244" s="10"/>
       <c r="C244" s="10"/>
@@ -8074,7 +8046,7 @@
       <c r="X244" s="10"/>
       <c r="Y244" s="10"/>
     </row>
-    <row r="245" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="15"/>
       <c r="B245" s="10"/>
       <c r="C245" s="10"/>
@@ -8101,7 +8073,7 @@
       <c r="X245" s="10"/>
       <c r="Y245" s="10"/>
     </row>
-    <row r="246" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="15"/>
       <c r="B246" s="10"/>
       <c r="C246" s="10"/>
@@ -8128,7 +8100,7 @@
       <c r="X246" s="10"/>
       <c r="Y246" s="10"/>
     </row>
-    <row r="247" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="15"/>
       <c r="B247" s="10"/>
       <c r="C247" s="10"/>
@@ -8155,7 +8127,7 @@
       <c r="X247" s="10"/>
       <c r="Y247" s="10"/>
     </row>
-    <row r="248" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="15"/>
       <c r="B248" s="10"/>
       <c r="C248" s="10"/>
@@ -8182,7 +8154,7 @@
       <c r="X248" s="10"/>
       <c r="Y248" s="10"/>
     </row>
-    <row r="249" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="15"/>
       <c r="B249" s="10"/>
       <c r="C249" s="10"/>
@@ -8209,7 +8181,7 @@
       <c r="X249" s="10"/>
       <c r="Y249" s="10"/>
     </row>
-    <row r="250" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="15"/>
       <c r="B250" s="10"/>
       <c r="C250" s="10"/>
@@ -8236,7 +8208,7 @@
       <c r="X250" s="10"/>
       <c r="Y250" s="10"/>
     </row>
-    <row r="251" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="15"/>
       <c r="B251" s="10"/>
       <c r="C251" s="10"/>
@@ -8263,7 +8235,7 @@
       <c r="X251" s="10"/>
       <c r="Y251" s="10"/>
     </row>
-    <row r="252" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="15"/>
       <c r="B252" s="10"/>
       <c r="C252" s="10"/>
@@ -8290,754 +8262,754 @@
       <c r="X252" s="10"/>
       <c r="Y252" s="10"/>
     </row>
-    <row r="253" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>